<commit_message>
Correct `ExtractText` behaviour the following way:
- Linebreaks
  - For doc linebreak is being added after each paragraph
  - For pres linebreak is being added after each paragraph in each slide
  - For wb linebreak is being added after each row in each sheet
- Args
  - Added arg to wb's `ExtractText` - a slice containing sheets indexes
</commit_message>
<xml_diff>
--- a/spreadsheet/testdata/extraction.xlsx
+++ b/spreadsheet/testdata/extraction.xlsx
@@ -8,12 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/darkrengarius/go/src/test/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{6D34D439-9EF2-4E4C-B48A-F17D553A4428}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:9_{41550ADC-8458-614B-BBE9-03FDEE6865CD}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="15960" xr2:uid="{AF43583E-1547-A443-A8F9-3273BE256D9E}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="15960" activeTab="1" xr2:uid="{AF43583E-1547-A443-A8F9-3273BE256D9E}"/>
   </bookViews>
   <sheets>
     <sheet name="Лист1" sheetId="1" r:id="rId1"/>
+    <sheet name="Лист2" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -34,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" count="9" uniqueCount="8">
+<sst xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" count="14" uniqueCount="13">
   <si>
     <t>qwe</t>
   </si>
@@ -58,6 +59,21 @@
   </si>
   <si>
     <t>cbn</t>
+  </si>
+  <si>
+    <t>l21</t>
+  </si>
+  <si>
+    <t>l22</t>
+  </si>
+  <si>
+    <t>l23</t>
+  </si>
+  <si>
+    <t>l24</t>
+  </si>
+  <si>
+    <t>l25</t>
   </si>
 </sst>
 </file>
@@ -413,7 +429,7 @@
 <worksheet xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" xmlns:r="http://purl.oclc.org/ooxml/officeDocument/relationships" xmlns:v="urn:schemas-microsoft-com:vml" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{204D25EB-A7CA-DE44-BD43-FCEEDEBE1872}">
   <dimension ref="A1:J9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="L24" sqref="L24"/>
     </sheetView>
   </sheetViews>
@@ -472,4 +488,42 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" xmlns:r="http://purl.oclc.org/ooxml/officeDocument/relationships" xmlns:v="urn:schemas-microsoft-com:vml" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C9883832-280C-844D-AC50-345400B1FE75}">
+  <dimension ref="A1:E5"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E6" sqref="E6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B3" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="C4" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="D5" t="s">
+        <v>11</v>
+      </c>
+      <c r="E5" t="s">
+        <v>12</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>